<commit_message>
updates to the document.
</commit_message>
<xml_diff>
--- a/documents/sdr-release-2.0/usdm-v1.9-model-changes-conformance-rules.xlsx
+++ b/documents/sdr-release-2.0/usdm-v1.9-model-changes-conformance-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ts.accenture.com/sites/DigitalDataFlow-ACNOnly/Shared Documents/ACN Only/Phase 1/SDR V2.0 Release (Aug-2022-Mar-2023)/01 - Sprint Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indu.sekhar.sajja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="559" documentId="13_ncr:1_{A981E9CA-A239-49F2-BDD2-AC41A1C7BDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9628DF9A-5E5B-4687-A372-8E0E61F47C6C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB8A881D-3431-4FF3-B1F1-FEB164488AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{A3ACD5DA-FA69-451A-83B4-E2EA342D7D58}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4619" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4603" uniqueCount="516">
   <si>
     <t>StudyElement</t>
   </si>
@@ -1220,30 +1220,6 @@
     <t>Attribute is marked non-mandatory</t>
   </si>
   <si>
-    <t>Sprint2</t>
-  </si>
-  <si>
-    <t>Sprint3</t>
-  </si>
-  <si>
-    <t>Sprint4</t>
-  </si>
-  <si>
-    <t>Sprint5</t>
-  </si>
-  <si>
-    <t>Sprint6</t>
-  </si>
-  <si>
-    <t>Sprint7</t>
-  </si>
-  <si>
-    <t>Sprint8</t>
-  </si>
-  <si>
-    <t>Sprint9</t>
-  </si>
-  <si>
     <t>Attribute is marked non-mandatory, Type changed from treatment--&gt;InvestigationalIntervention</t>
   </si>
   <si>
@@ -1352,9 +1328,6 @@
     <t>scheduleTimelineEntryId</t>
   </si>
   <si>
-    <t>Cross-Reference to ScheduledInstance</t>
-  </si>
-  <si>
     <t>scheduleTimelineExits</t>
   </si>
   <si>
@@ -1376,15 +1349,9 @@
     <t>scheduleTimelineExitId</t>
   </si>
   <si>
-    <t>Cross-Reference to ScheduleTimelineExit</t>
-  </si>
-  <si>
     <t>scheduledInstanceEncounterId</t>
   </si>
   <si>
-    <t>Cross-Reference to Encounter</t>
-  </si>
-  <si>
     <t>scheduleSeqenceNumber</t>
   </si>
   <si>
@@ -1397,9 +1364,6 @@
     <t>scheduleInstanceTimelineId</t>
   </si>
   <si>
-    <t>Cross-Reference to ScheduledTimeline</t>
-  </si>
-  <si>
     <t>scheduledInstanceType</t>
   </si>
   <si>
@@ -1409,18 +1373,12 @@
     <t>activityIds</t>
   </si>
   <si>
-    <t>Will be considered when scheduledInstanceType = ACTIVITY &amp; Cross-Reference to Activities</t>
-  </si>
-  <si>
     <t>conditionAssignments</t>
   </si>
   <si>
     <t>Dictionary&lt;string,string&gt;</t>
   </si>
   <si>
-    <t>Will be considered when scheduledInstanceType = DECISION</t>
-  </si>
-  <si>
     <t>Timing</t>
   </si>
   <si>
@@ -1674,6 +1632,30 @@
   </si>
   <si>
     <t>Attribute Removed</t>
+  </si>
+  <si>
+    <t>New Class (TimePoints)
+1. scheduleTimelineEntryId - Cross-Reference to ScheduledInstance</t>
+  </si>
+  <si>
+    <t>New Class (TimePoints)
+1. scheduleTimelineExitId - Cross-Reference to ScheduleTimelineExit
+2. scheduledInstanceEncounterId - Cross-Reference to Encounter
+3. scheduleInstanceTimelineId - Cross-Reference to ScheduledTimeline
+4. activityIds attribute will be considered only when scheduledInstanceType = ACTIVITY &amp; Cross-References to Activity
+5. conditionAssignments attribute will be considered only when scheduledInstanceType = DECISION</t>
+  </si>
+  <si>
+    <t>New Class (TimePoints)
+1. relativeToScheduledInstanceId - Cross-Reference to ScheduledInstance
+2. relativeFromScheduledInstanceId - Cross-Reference to ScheduledInstance</t>
+  </si>
+  <si>
+    <t>Attribute name changed Desc--&gt; Description</t>
+  </si>
+  <si>
+    <t>New Class (Biomedical Concepts)
+1. bcCategoryMemberIds - Cross-Reference to biomedicalConcept</t>
   </si>
 </sst>
 </file>
@@ -1759,7 +1741,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1811,12 +1793,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1964,7 +1940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2095,7 +2071,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2129,13 +2104,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3031,7 +3008,7 @@
         <v>36</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>376</v>
@@ -3046,7 +3023,7 @@
         <v>36</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>376</v>
@@ -3962,7 +3939,7 @@
         <v>151</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -4187,10 +4164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F0EAED-8561-4EDA-A107-AA21EA320644}">
-  <dimension ref="A1:F199"/>
+  <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E189" sqref="E189"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4199,8 +4176,7 @@
     <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="79.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -4237,7 +4213,7 @@
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>9</v>
@@ -4250,7 +4226,7 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>9</v>
@@ -4272,11 +4248,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B6" s="62"/>
       <c r="C6" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D6" s="62" t="s">
         <v>9</v>
@@ -4287,11 +4263,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B7" s="62"/>
       <c r="C7" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D7" s="62" t="s">
         <v>9</v>
@@ -4321,7 +4297,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D9" s="51" t="s">
         <v>18</v>
@@ -4336,7 +4312,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>9</v>
@@ -4364,7 +4340,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>18</v>
@@ -4379,7 +4355,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>9</v>
@@ -4392,7 +4368,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>9</v>
@@ -4405,7 +4381,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>9</v>
@@ -4428,10 +4404,10 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="29"/>
       <c r="B17" s="62" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="D17" s="62" t="s">
         <v>6</v>
@@ -4446,13 +4422,13 @@
       </c>
       <c r="B18" s="54"/>
       <c r="C18" s="54" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D18" s="54" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -4476,7 +4452,7 @@
         <v>30</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>18</v>
@@ -4491,7 +4467,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>9</v>
@@ -4504,7 +4480,7 @@
         <v>32</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>9</v>
@@ -4517,7 +4493,7 @@
         <v>38</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D23" s="27" t="s">
         <v>9</v>
@@ -4530,7 +4506,7 @@
         <v>39</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D24" s="27" t="s">
         <v>9</v>
@@ -4543,7 +4519,7 @@
         <v>37</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>9</v>
@@ -4556,7 +4532,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>6</v>
@@ -4569,7 +4545,7 @@
         <v>34</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D27" s="27" t="s">
         <v>9</v>
@@ -4625,7 +4601,7 @@
         <v>44</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>18</v>
@@ -4640,7 +4616,7 @@
         <v>45</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D32" s="27" t="s">
         <v>9</v>
@@ -4652,7 +4628,7 @@
         <v>46</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D33" s="27" t="s">
         <v>9</v>
@@ -4667,7 +4643,7 @@
         <v>36</v>
       </c>
       <c r="D34" s="53" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E34" s="51" t="s">
         <v>376</v>
@@ -4682,7 +4658,7 @@
         <v>36</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E35" s="51" t="s">
         <v>376</v>
@@ -4776,22 +4752,22 @@
         <v>6</v>
       </c>
       <c r="E42" s="54" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="31"/>
       <c r="B43" s="47" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C43" s="47" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="D43" s="47" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="47" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -4840,10 +4816,10 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
       <c r="B47" s="62" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C47" s="62" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="D47" s="62" t="s">
         <v>6</v>
@@ -4855,10 +4831,10 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="31"/>
       <c r="B48" s="62" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C48" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D48" s="62" t="s">
         <v>9</v>
@@ -4870,10 +4846,10 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="31"/>
       <c r="B49" s="62" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D49" s="62" t="s">
         <v>6</v>
@@ -4885,46 +4861,46 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="31"/>
       <c r="B50" s="62" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C50" s="62" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="D50" s="62" t="s">
         <v>6</v>
       </c>
       <c r="E50" s="62" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="31"/>
       <c r="B51" s="62" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D51" s="62" t="s">
         <v>6</v>
       </c>
       <c r="E51" s="62" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="31"/>
       <c r="B52" s="62" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C52" s="62" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="D52" s="62" t="s">
         <v>6</v>
       </c>
       <c r="E52" s="62" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -4935,7 +4911,7 @@
         <v>66</v>
       </c>
       <c r="C53" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D53" s="51" t="s">
         <v>18</v>
@@ -4991,7 +4967,7 @@
         <v>71</v>
       </c>
       <c r="C57" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D57" s="51" t="s">
         <v>18</v>
@@ -5006,7 +4982,7 @@
         <v>76</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D58" s="27" t="s">
         <v>9</v>
@@ -5019,13 +4995,13 @@
         <v>75</v>
       </c>
       <c r="C59" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D59" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E59" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -5047,13 +5023,13 @@
         <v>72</v>
       </c>
       <c r="C61" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D61" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E61" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -5077,7 +5053,7 @@
         <v>79</v>
       </c>
       <c r="C63" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D63" s="51" t="s">
         <v>18</v>
@@ -5092,7 +5068,7 @@
         <v>81</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D64" s="27" t="s">
         <v>9</v>
@@ -5105,13 +5081,13 @@
         <v>80</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D65" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E65" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -5148,7 +5124,7 @@
         <v>85</v>
       </c>
       <c r="C68" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D68" s="51" t="s">
         <v>18</v>
@@ -5161,7 +5137,7 @@
         <v>90</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D69" s="27" t="s">
         <v>9</v>
@@ -5174,13 +5150,13 @@
         <v>89</v>
       </c>
       <c r="C70" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D70" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E70" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -5202,13 +5178,13 @@
         <v>88</v>
       </c>
       <c r="C72" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D72" s="51" t="s">
         <v>18</v>
       </c>
       <c r="E72" s="51" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -5217,28 +5193,28 @@
         <v>86</v>
       </c>
       <c r="C73" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D73" s="51" t="s">
         <v>18</v>
       </c>
       <c r="E73" s="51" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="28"/>
-      <c r="B74" s="82" t="s">
+      <c r="B74" s="80" t="s">
         <v>92</v>
       </c>
       <c r="C74" s="54" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D74" s="54" t="s">
         <v>6</v>
       </c>
       <c r="E74" s="55" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -5249,7 +5225,7 @@
         <v>95</v>
       </c>
       <c r="C75" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D75" s="51" t="s">
         <v>18</v>
@@ -5264,13 +5240,13 @@
         <v>97</v>
       </c>
       <c r="C76" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D76" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E76" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -5294,7 +5270,7 @@
         <v>99</v>
       </c>
       <c r="C78" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D78" s="51" t="s">
         <v>18</v>
@@ -5309,7 +5285,7 @@
         <v>100</v>
       </c>
       <c r="C79" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D79" s="27" t="s">
         <v>9</v>
@@ -5337,7 +5313,7 @@
         <v>102</v>
       </c>
       <c r="C81" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D81" s="51" t="s">
         <v>18</v>
@@ -5352,13 +5328,13 @@
         <v>103</v>
       </c>
       <c r="C82" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D82" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E82" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -5395,7 +5371,7 @@
         <v>108</v>
       </c>
       <c r="C85" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D85" s="51" t="s">
         <v>18</v>
@@ -5410,13 +5386,13 @@
         <v>109</v>
       </c>
       <c r="C86" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D86" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E86" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
@@ -5425,13 +5401,13 @@
         <v>111</v>
       </c>
       <c r="C87" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D87" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E87" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -5455,7 +5431,7 @@
         <v>113</v>
       </c>
       <c r="C89" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D89" s="51" t="s">
         <v>18</v>
@@ -5470,22 +5446,22 @@
         <v>114</v>
       </c>
       <c r="C90" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D90" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E90" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="28"/>
       <c r="B91" s="62" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C91" s="62" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="D91" s="62" t="s">
         <v>9</v>
@@ -5497,10 +5473,10 @@
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="28"/>
       <c r="B92" s="62" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C92" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D92" s="62" t="s">
         <v>9</v>
@@ -5512,10 +5488,10 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="28"/>
       <c r="B93" s="62" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C93" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D93" s="62" t="s">
         <v>9</v>
@@ -5527,7 +5503,7 @@
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="28"/>
       <c r="B94" s="62" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C94" s="62" t="s">
         <v>36</v>
@@ -5547,13 +5523,13 @@
         <v>116</v>
       </c>
       <c r="C95" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D95" s="53" t="s">
         <v>9</v>
       </c>
       <c r="E95" s="58" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -5562,14 +5538,14 @@
         <v>117</v>
       </c>
       <c r="C96" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D96" s="53" t="s">
         <v>9</v>
       </c>
       <c r="E96" s="59"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="57"/>
       <c r="B97" s="53" t="s">
         <v>118</v>
@@ -5582,7 +5558,7 @@
       </c>
       <c r="E97" s="60"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="56" t="s">
         <v>120</v>
       </c>
@@ -5590,342 +5566,317 @@
         <v>121</v>
       </c>
       <c r="C98" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D98" s="53" t="s">
         <v>9</v>
       </c>
       <c r="E98" s="58" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="56"/>
       <c r="B99" s="53" t="s">
         <v>124</v>
       </c>
       <c r="C99" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D99" s="53" t="s">
         <v>9</v>
       </c>
       <c r="E99" s="59"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="56"/>
       <c r="B100" s="53" t="s">
         <v>128</v>
       </c>
       <c r="C100" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D100" s="53" t="s">
         <v>6</v>
       </c>
       <c r="E100" s="59"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="56"/>
       <c r="B101" s="53" t="s">
         <v>127</v>
       </c>
       <c r="C101" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D101" s="53" t="s">
         <v>6</v>
       </c>
       <c r="E101" s="59"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="56"/>
       <c r="B102" s="53" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="C102" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D102" s="53" t="s">
         <v>6</v>
       </c>
       <c r="E102" s="59"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="56"/>
       <c r="B103" s="53" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="C103" s="53" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D103" s="53" t="s">
         <v>6</v>
       </c>
       <c r="E103" s="60"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="63" t="s">
-        <v>411</v>
-      </c>
-      <c r="B104" s="69" t="s">
-        <v>412</v>
+        <v>403</v>
+      </c>
+      <c r="B104" s="68" t="s">
+        <v>404</v>
       </c>
       <c r="C104" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D104" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E104" s="71" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E104" s="82" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="63"/>
-      <c r="B105" s="69" t="s">
-        <v>413</v>
+      <c r="B105" s="68" t="s">
+        <v>405</v>
       </c>
       <c r="C105" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D105" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E105" s="72"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E105" s="71"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="63"/>
-      <c r="B106" s="69" t="s">
-        <v>414</v>
+      <c r="B106" s="68" t="s">
+        <v>406</v>
       </c>
       <c r="C106" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D106" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E106" s="72"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E106" s="71"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="63"/>
-      <c r="B107" s="69" t="s">
-        <v>415</v>
+      <c r="B107" s="68" t="s">
+        <v>407</v>
       </c>
       <c r="C107" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D107" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E107" s="72"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E107" s="71"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="63"/>
-      <c r="B108" s="69" t="s">
-        <v>416</v>
+      <c r="B108" s="68" t="s">
+        <v>408</v>
       </c>
       <c r="C108" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D108" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E108" s="72"/>
-      <c r="F108" s="64" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E108" s="71"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="63"/>
-      <c r="B109" s="69" t="s">
-        <v>418</v>
+      <c r="B109" s="68" t="s">
+        <v>409</v>
       </c>
       <c r="C109" s="62" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D109" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E109" s="72"/>
-      <c r="F109" s="64"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E109" s="71"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="63"/>
-      <c r="B110" s="69" t="s">
-        <v>420</v>
+      <c r="B110" s="68" t="s">
+        <v>411</v>
       </c>
       <c r="C110" s="62" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D110" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E110" s="73"/>
-      <c r="F110" s="64"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A111" s="65" t="s">
-        <v>422</v>
-      </c>
-      <c r="B111" s="70" t="s">
-        <v>423</v>
+      <c r="E110" s="72"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" s="64" t="s">
+        <v>413</v>
+      </c>
+      <c r="B111" s="69" t="s">
+        <v>414</v>
       </c>
       <c r="C111" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D111" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E111" s="71" t="s">
-        <v>514</v>
-      </c>
-      <c r="F111" s="64"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A112" s="65"/>
+      <c r="E111" s="82" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="64"/>
       <c r="B112" s="62" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="C112" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D112" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E112" s="72"/>
-      <c r="F112" s="64" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A113" s="65"/>
+      <c r="E112" s="71"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" s="64"/>
       <c r="B113" s="62" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="C113" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D113" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E113" s="72"/>
-      <c r="F113" s="64" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A114" s="65"/>
+      <c r="E113" s="71"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="64"/>
       <c r="B114" s="62" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="C114" s="62" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="D114" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E114" s="72"/>
-      <c r="F114" s="64"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A115" s="65"/>
+      <c r="E114" s="71"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" s="64"/>
       <c r="B115" s="62" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="C115" s="62" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="D115" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="72"/>
-      <c r="F115" s="64"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A116" s="65"/>
+      <c r="E115" s="71"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" s="64"/>
       <c r="B116" s="62" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="C116" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D116" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E116" s="72"/>
-      <c r="F116" s="64" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A117" s="65"/>
+      <c r="E116" s="71"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="64"/>
       <c r="B117" s="62" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="C117" s="62" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D117" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E117" s="72"/>
-      <c r="F117" s="64"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A118" s="65"/>
+      <c r="E117" s="71"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="64"/>
       <c r="B118" s="62" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="C118" s="62" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D118" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="72"/>
-      <c r="F118" s="64" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A119" s="65"/>
+      <c r="E118" s="71"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="64"/>
       <c r="B119" s="62" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="C119" s="62" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="D119" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E119" s="73"/>
-      <c r="F119" s="64" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A120" s="66" t="s">
-        <v>440</v>
+      <c r="E119" s="72"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" s="65" t="s">
+        <v>426</v>
       </c>
       <c r="B120" s="62" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="C120" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D120" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E120" s="71" t="s">
-        <v>514</v>
-      </c>
-      <c r="F120" s="64"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A121" s="65"/>
+      <c r="E120" s="82" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" s="64"/>
       <c r="B121" s="62" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="C121" s="62" t="s">
         <v>12</v>
@@ -5933,99 +5884,91 @@
       <c r="D121" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E121" s="72"/>
-      <c r="F121" s="64"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A122" s="65"/>
+      <c r="E121" s="71"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" s="64"/>
       <c r="B122" s="62" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="C122" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D122" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E122" s="72"/>
-      <c r="F122" s="64"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A123" s="65"/>
+      <c r="E122" s="71"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" s="64"/>
       <c r="B123" s="62" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="C123" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D123" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E123" s="72"/>
-      <c r="F123" s="64" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A124" s="65"/>
+      <c r="E123" s="71"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" s="64"/>
       <c r="B124" s="62" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="C124" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D124" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E124" s="72"/>
-      <c r="F124" s="64" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A125" s="65"/>
+      <c r="E124" s="71"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" s="64"/>
       <c r="B125" s="62" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="C125" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D125" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="72"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A126" s="67"/>
+      <c r="E125" s="71"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" s="66"/>
       <c r="B126" s="62" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="C126" s="62" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="D126" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E126" s="73"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A127" s="68" t="s">
-        <v>449</v>
+      <c r="E126" s="72"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" s="67" t="s">
+        <v>435</v>
       </c>
       <c r="B127" s="62" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="C127" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D127" s="62" t="s">
         <v>9</v>
       </c>
       <c r="E127" s="62" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="31" t="s">
         <v>123</v>
       </c>
@@ -6033,7 +5976,7 @@
         <v>129</v>
       </c>
       <c r="C128" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D128" s="51" t="s">
         <v>18</v>
@@ -6048,7 +5991,7 @@
         <v>131</v>
       </c>
       <c r="C129" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D129" s="27" t="s">
         <v>9</v>
@@ -6061,13 +6004,13 @@
         <v>130</v>
       </c>
       <c r="C130" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D130" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E130" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -6076,7 +6019,7 @@
         <v>135</v>
       </c>
       <c r="C131" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D131" s="27" t="s">
         <v>6</v>
@@ -6089,7 +6032,7 @@
         <v>134</v>
       </c>
       <c r="C132" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D132" s="27" t="s">
         <v>6</v>
@@ -6121,16 +6064,16 @@
         <v>6</v>
       </c>
       <c r="E134" s="54" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="31"/>
       <c r="B135" s="62" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="C135" s="62" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D135" s="62" t="s">
         <v>9</v>
@@ -6142,10 +6085,10 @@
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="31"/>
       <c r="B136" s="62" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="C136" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D136" s="62" t="s">
         <v>9</v>
@@ -6157,61 +6100,61 @@
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="31"/>
       <c r="B137" s="62" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="C137" s="62" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D137" s="62" t="s">
         <v>6</v>
       </c>
       <c r="E137" s="62" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="31"/>
       <c r="B138" s="62" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="C138" s="62" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D138" s="62" t="s">
         <v>6</v>
       </c>
       <c r="E138" s="62" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="31"/>
       <c r="B139" s="62" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="C139" s="62" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D139" s="62" t="s">
         <v>6</v>
       </c>
       <c r="E139" s="62" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="31"/>
       <c r="B140" s="47" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="C140" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D140" s="47" t="s">
         <v>6</v>
       </c>
       <c r="E140" s="47" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -6222,7 +6165,7 @@
         <v>139</v>
       </c>
       <c r="C141" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D141" s="51" t="s">
         <v>18</v>
@@ -6237,7 +6180,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D142" s="27" t="s">
         <v>9</v>
@@ -6259,10 +6202,10 @@
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="33"/>
       <c r="B144" s="62" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="C144" s="62" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D144" s="62" t="s">
         <v>9</v>
@@ -6274,10 +6217,10 @@
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="34"/>
       <c r="B145" s="62" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="C145" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D145" s="62" t="s">
         <v>9</v>
@@ -6290,57 +6233,57 @@
       <c r="A146" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B146" s="74" t="s">
+      <c r="B146" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="C146" s="74" t="s">
-        <v>387</v>
-      </c>
-      <c r="D146" s="74" t="s">
+      <c r="C146" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="D146" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E146" s="75" t="s">
-        <v>511</v>
+      <c r="E146" s="74" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="42"/>
-      <c r="B147" s="74" t="s">
+      <c r="B147" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="C147" s="74" t="s">
-        <v>387</v>
-      </c>
-      <c r="D147" s="74" t="s">
+      <c r="C147" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="D147" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="E147" s="76"/>
+      <c r="E147" s="75"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="42"/>
-      <c r="B148" s="74" t="s">
+      <c r="B148" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="C148" s="74" t="s">
-        <v>387</v>
-      </c>
-      <c r="D148" s="74" t="s">
+      <c r="C148" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="D148" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="E148" s="76"/>
+      <c r="E148" s="75"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="42"/>
-      <c r="B149" s="74" t="s">
+      <c r="B149" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="C149" s="74" t="s">
-        <v>387</v>
-      </c>
-      <c r="D149" s="74" t="s">
+      <c r="C149" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="D149" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="E149" s="77"/>
+      <c r="E149" s="76"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="35" t="s">
@@ -6350,7 +6293,7 @@
         <v>149</v>
       </c>
       <c r="C150" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D150" s="51" t="s">
         <v>18</v>
@@ -6365,7 +6308,7 @@
         <v>152</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D151" s="27" t="s">
         <v>9</v>
@@ -6390,13 +6333,13 @@
         <v>150</v>
       </c>
       <c r="C153" s="54" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D153" s="51" t="s">
         <v>151</v>
       </c>
       <c r="E153" s="51" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -6405,13 +6348,13 @@
         <v>154</v>
       </c>
       <c r="C154" s="54" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D154" s="51" t="s">
         <v>151</v>
       </c>
       <c r="E154" s="51" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
@@ -6435,7 +6378,7 @@
         <v>157</v>
       </c>
       <c r="C156" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D156" s="51" t="s">
         <v>18</v>
@@ -6450,13 +6393,13 @@
         <v>114</v>
       </c>
       <c r="C157" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D157" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E157" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
@@ -6467,7 +6410,7 @@
         <v>159</v>
       </c>
       <c r="C158" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D158" s="51" t="s">
         <v>18</v>
@@ -6482,7 +6425,7 @@
         <v>161</v>
       </c>
       <c r="C159" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D159" s="27" t="s">
         <v>9</v>
@@ -6495,13 +6438,13 @@
         <v>160</v>
       </c>
       <c r="C160" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D160" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E160" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
@@ -6510,7 +6453,7 @@
         <v>162</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D161" s="27" t="s">
         <v>9</v>
@@ -6519,28 +6462,28 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="43" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="B162" s="47" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="C162" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D162" s="47" t="s">
         <v>9</v>
       </c>
       <c r="E162" s="43" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="45"/>
       <c r="B163" s="47" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="C163" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D163" s="47" t="s">
         <v>9</v>
@@ -6550,10 +6493,10 @@
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="45"/>
       <c r="B164" s="47" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="C164" s="47" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D164" s="47" t="s">
         <v>6</v>
@@ -6563,10 +6506,10 @@
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="45"/>
       <c r="B165" s="47" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="C165" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D165" s="47" t="s">
         <v>9</v>
@@ -6576,10 +6519,10 @@
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="45"/>
       <c r="B166" s="47" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="C166" s="47" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="D166" s="47" t="s">
         <v>6</v>
@@ -6589,10 +6532,10 @@
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="46"/>
       <c r="B167" s="47" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="C167" s="47" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D167" s="47" t="s">
         <v>9</v>
@@ -6601,28 +6544,28 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="48" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="B168" s="47" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="C168" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D168" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E168" s="43" t="s">
-        <v>510</v>
+      <c r="E168" s="48" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="49"/>
       <c r="B169" s="47" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="C169" s="47" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D169" s="47" t="s">
         <v>6</v>
@@ -6632,10 +6575,10 @@
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="49"/>
       <c r="B170" s="47" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C170" s="47" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D170" s="47" t="s">
         <v>6</v>
@@ -6645,10 +6588,10 @@
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="49"/>
       <c r="B171" s="47" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="C171" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D171" s="47" t="s">
         <v>9</v>
@@ -6658,10 +6601,10 @@
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="49"/>
       <c r="B172" s="47" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="C172" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D172" s="47" t="s">
         <v>9</v>
@@ -6671,10 +6614,10 @@
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="50"/>
       <c r="B173" s="47" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="C173" s="47" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D173" s="47" t="s">
         <v>6</v>
@@ -6683,28 +6626,28 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="43" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="B174" s="47" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="C174" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D174" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E174" s="43" t="s">
-        <v>510</v>
+      <c r="E174" s="48" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="45"/>
       <c r="B175" s="47" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="C175" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D175" s="47" t="s">
         <v>9</v>
@@ -6714,10 +6657,10 @@
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="45"/>
       <c r="B176" s="47" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="C176" s="47" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D176" s="47" t="s">
         <v>9</v>
@@ -6727,10 +6670,10 @@
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="45"/>
       <c r="B177" s="47" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="C177" s="47" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D177" s="47" t="s">
         <v>9</v>
@@ -6740,10 +6683,10 @@
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="45"/>
       <c r="B178" s="47" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="C178" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D178" s="47" t="s">
         <v>9</v>
@@ -6753,10 +6696,10 @@
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="45"/>
       <c r="B179" s="47" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="C179" s="47" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="D179" s="47" t="s">
         <v>6</v>
@@ -6766,10 +6709,10 @@
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="46"/>
       <c r="B180" s="47" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="C180" s="47" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D180" s="47" t="s">
         <v>9</v>
@@ -6778,28 +6721,28 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="43" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B181" s="47" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="C181" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D181" s="47" t="s">
         <v>9</v>
       </c>
       <c r="E181" s="43" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="45"/>
       <c r="B182" s="47" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="C182" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D182" s="47" t="s">
         <v>9</v>
@@ -6809,10 +6752,10 @@
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="45"/>
       <c r="B183" s="47" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="C183" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D183" s="47" t="s">
         <v>9</v>
@@ -6822,10 +6765,10 @@
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="46"/>
       <c r="B184" s="47" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="C184" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D184" s="47" t="s">
         <v>9</v>
@@ -6834,28 +6777,28 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="43" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="B185" s="47" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="C185" s="47" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D185" s="47" t="s">
         <v>9</v>
       </c>
       <c r="E185" s="43" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="45"/>
       <c r="B186" s="47" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="C186" s="47" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D186" s="47" t="s">
         <v>9</v>
@@ -6874,46 +6817,6 @@
         <v>9</v>
       </c>
       <c r="E187" s="46"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A192" s="78" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A193" s="78" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A194" s="78" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A195" s="78" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A196" s="78" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A197" s="78" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
-        <v>384</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -7305,7 +7208,7 @@
         <v>165</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D2" s="51" t="s">
         <v>18</v>
@@ -7320,7 +7223,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>9</v>
@@ -7333,7 +7236,7 @@
         <v>166</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>9</v>
@@ -7346,7 +7249,7 @@
         <v>167</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>9</v>
@@ -7359,7 +7262,7 @@
         <v>168</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>9</v>
@@ -7374,7 +7277,7 @@
         <v>169</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D7" s="51" t="s">
         <v>18</v>
@@ -7389,13 +7292,13 @@
         <v>170</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D8" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -7406,7 +7309,7 @@
         <v>171</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D9" s="51" t="s">
         <v>18</v>
@@ -7421,7 +7324,7 @@
         <v>175</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>9</v>
@@ -7434,13 +7337,13 @@
         <v>173</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>73</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -7449,7 +7352,7 @@
         <v>178</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
@@ -7462,7 +7365,7 @@
         <v>177</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -7497,8 +7400,8 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
-      <c r="B16" s="83" t="s">
-        <v>494</v>
+      <c r="B16" s="81" t="s">
+        <v>480</v>
       </c>
       <c r="C16" s="52" t="s">
         <v>36</v>
@@ -7507,7 +7410,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="51" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -7538,40 +7441,40 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="38"/>
-      <c r="B19" s="79" t="s">
-        <v>495</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>387</v>
-      </c>
-      <c r="D19" s="79" t="s">
+      <c r="B19" s="77" t="s">
+        <v>481</v>
+      </c>
+      <c r="C19" s="77" t="s">
+        <v>379</v>
+      </c>
+      <c r="D19" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="79" t="s">
-        <v>520</v>
+      <c r="E19" s="77" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="31" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="C20" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D20" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="71" t="s">
-        <v>509</v>
+      <c r="E20" s="70" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="40"/>
       <c r="B21" s="62" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>12</v>
@@ -7579,107 +7482,107 @@
       <c r="D21" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="72"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="40"/>
-      <c r="B22" s="80" t="s">
-        <v>499</v>
-      </c>
-      <c r="C22" s="81" t="s">
+      <c r="B22" s="78" t="s">
+        <v>485</v>
+      </c>
+      <c r="C22" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="80" t="s">
+      <c r="D22" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="73"/>
+      <c r="E22" s="72"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="31" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="C23" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D23" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="71" t="s">
-        <v>509</v>
+      <c r="E23" s="70" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="40"/>
       <c r="B24" s="62" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D24" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="72"/>
+      <c r="E24" s="71"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="40"/>
       <c r="B25" s="62" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D25" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="72"/>
+      <c r="E25" s="71"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="40"/>
       <c r="B26" s="62" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D26" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="72"/>
+      <c r="E26" s="71"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="40"/>
       <c r="B27" s="62" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D27" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="72"/>
+      <c r="E27" s="71"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="40"/>
       <c r="B28" s="62" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D28" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="72"/>
+      <c r="E28" s="71"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="41"/>
       <c r="B29" s="62" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="C29" s="62" t="s">
         <v>12</v>
@@ -7687,7 +7590,7 @@
       <c r="D29" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="73"/>
+      <c r="E29" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -19535,4 +19438,10 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>